<commit_message>
Add E-Paper Example Guides  for AmebaD
- Add E-Paper Example Guide for AmebaD
- Delete SPI and E-paper from bak folder
- Modify AMBD common excel
</commit_message>
<xml_diff>
--- a/bak/ambd/AMBD_common_example.xlsx
+++ b/bak/ambd/AMBD_common_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuenkaifai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDK_GitHub_Pammy_Repo\For_commit\dev\ameba-arduino-doc\bak\ambd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE27985-317F-411B-AAF5-A5AAE413AEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF78B0-A323-4139-8DA2-228063ABBB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{723630AB-5CF6-45CE-8453-96D6B2D408C1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{723630AB-5CF6-45CE-8453-96D6B2D408C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,13 +519,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -894,17 +894,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04CD4947-CD01-4C8D-9670-22AF8630FC97}">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J87" sqref="J87"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70:G70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -927,7 +927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -950,7 +950,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -973,7 +973,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -996,7 +996,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>68</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>69</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>74</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
@@ -2502,19 +2502,19 @@
         <v>94</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>95</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>96</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>83</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>84</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>97</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>98</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>99</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>100</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>89</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>91</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Add FAQ questions and E-Paper Guide for AMBD (#33)
* Add FAQ questions

Add FAQ questions

* Add E-Paper Example Guides  for AmebaD

- Add E-Paper Example Guide for AmebaD
- Delete SPI and E-paper from bak folder
- Modify AMBD common excel

* Update ebook images

Update ebook images
</commit_message>
<xml_diff>
--- a/bak/ambd/AMBD_common_example.xlsx
+++ b/bak/ambd/AMBD_common_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuenkaifai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDK_GitHub_Pammy_Repo\For_commit\dev\ameba-arduino-doc\bak\ambd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE27985-317F-411B-AAF5-A5AAE413AEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF78B0-A323-4139-8DA2-228063ABBB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{723630AB-5CF6-45CE-8453-96D6B2D408C1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{723630AB-5CF6-45CE-8453-96D6B2D408C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,13 +519,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -894,17 +894,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04CD4947-CD01-4C8D-9670-22AF8630FC97}">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J87" sqref="J87"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70:G70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -927,7 +927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -950,7 +950,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -973,7 +973,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -996,7 +996,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>68</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>69</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>74</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
@@ -2502,19 +2502,19 @@
         <v>94</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>95</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>96</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>83</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>84</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>97</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>98</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>99</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>100</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>89</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>91</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>93</v>
       </c>

</xml_diff>